<commit_message>
Increased push button indications reliability and command table
</commit_message>
<xml_diff>
--- a/questions/Assignment 8&9 - Blue Gecko Command Table.xlsx
+++ b/questions/Assignment 8&9 - Blue Gecko Command Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohit\SimplicityStudio\v4_workspace\ecen5823-assignments\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC739AC0-7BE1-4DB2-8D16-48DD2B2F5AA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7935368-2480-4AA3-8735-0C93DAF74952}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 67 Without Bonding" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="146">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -202,9 +202,6 @@
     <t>GATT_WAITING_FOR_CHARACTERISTICS_DISCOVERY</t>
   </si>
   <si>
-    <t>Searches for HTP temp measurement characteristic on attached server</t>
-  </si>
-  <si>
     <t>Saves characteristic handle in global strtuct</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>connection handle from evt_gatt_procedure_completed, characteristic handle from evt_gatt_characteristic (global state), flags gatt_indication</t>
   </si>
   <si>
-    <t>Sets up client for indications on HTP temp measurement change (only needed once per connection)</t>
-  </si>
-  <si>
     <t>"Handling Indications"</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>connection handle from evt_gatt_characteristic_value</t>
   </si>
   <si>
-    <t>Parses HTP temperature attribute from server and logs value, sends indication when necessary</t>
-  </si>
-  <si>
     <t>evt_le_connection_closed</t>
   </si>
   <si>
@@ -439,18 +430,6 @@
     <t>gecko_evt_gatt_characteristic_value</t>
   </si>
   <si>
-    <t>"Button State: X"</t>
-  </si>
-  <si>
-    <t>Assignment 9 - additional</t>
-  </si>
-  <si>
-    <t>Assignment 8 - additional</t>
-  </si>
-  <si>
-    <t>Sending cmd_sm_passkey_confirmation to server</t>
-  </si>
-  <si>
     <t>same as above for this state</t>
   </si>
   <si>
@@ -458,6 +437,27 @@
   </si>
   <si>
     <t>cmd_sm_delete_bondings, cmd_sm_configure, cmd_sm_set_bondable_mode, cmd_flash_ps_erase_all</t>
+  </si>
+  <si>
+    <t>Sending cmd_sm_passkey_confirmation to server; passkey confirm command executed in gecko_external event (button press interrupt)</t>
+  </si>
+  <si>
+    <t>Parses HTP temperature attribute and push button status from server and logs value, sends indication when necessary</t>
+  </si>
+  <si>
+    <t>Sets up client for indications on HTP temp measurement and push button status change (only needed once per connection)</t>
+  </si>
+  <si>
+    <t>Searches for HTP temp measurement and push button characteristic on attached server</t>
+  </si>
+  <si>
+    <t>Assignment 8 - additional server commands</t>
+  </si>
+  <si>
+    <t>Assignment 9 - additional server commands</t>
+  </si>
+  <si>
+    <t>"Button Pressed"/"Button Released"</t>
   </si>
 </sst>
 </file>
@@ -977,9 +977,9 @@
   </sheetPr>
   <dimension ref="A1:AJ976"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1499,8 +1499,8 @@
       <c r="M9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>60</v>
+      <c r="N9" s="5" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="13.2">
@@ -1544,7 +1544,7 @@
         <v>18</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:36" ht="39.6">
@@ -1558,16 +1558,16 @@
         <v>19</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>18</v>
@@ -1582,13 +1582,13 @@
         <v>47</v>
       </c>
       <c r="L11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>68</v>
+      <c r="N11" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:36" ht="39.6">
@@ -1614,49 +1614,49 @@
         <v>18</v>
       </c>
       <c r="H12" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="N12" s="8" t="s">
         <v>69</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="N12" s="8" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:36" ht="13.2">
       <c r="A13" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="G13" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>76</v>
-      </c>
       <c r="H13" s="12" t="s">
         <v>18</v>
       </c>
@@ -1675,16 +1675,16 @@
       <c r="M13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="N13" s="8" t="s">
-        <v>77</v>
+      <c r="N13" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:36" ht="26.4">
       <c r="A14" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>16</v>
@@ -1725,10 +1725,10 @@
     </row>
     <row r="15" spans="1:36" ht="26.4">
       <c r="A15" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>19</v>
@@ -1769,66 +1769,66 @@
     </row>
     <row r="16" spans="1:36" ht="13.2">
       <c r="A16" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="13.2">
       <c r="A17" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>18</v>
@@ -1852,30 +1852,30 @@
         <v>18</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="26.4">
       <c r="A18" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>18</v>
@@ -1884,7 +1884,7 @@
         <v>18</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K18" s="5" t="s">
         <v>18</v>
@@ -1896,12 +1896,12 @@
         <v>18</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="13.2">
       <c r="A19" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1919,25 +1919,25 @@
     </row>
     <row r="20" spans="1:14" ht="13.2">
       <c r="A20" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
@@ -1956,51 +1956,51 @@
         <v>18</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="13.2">
       <c r="A21" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="I21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="11" t="s">
+      <c r="L21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="13.2">
@@ -2021,7 +2021,7 @@
     </row>
     <row r="23" spans="1:14" ht="13.2">
       <c r="A23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="5"/>
@@ -2039,28 +2039,28 @@
     </row>
     <row r="24" spans="1:14" ht="13.2">
       <c r="A24" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>18</v>
@@ -2078,7 +2078,7 @@
         <v>18</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1">
@@ -2087,9 +2087,9 @@
     <row r="26" spans="1:14" ht="15.75" customHeight="1">
       <c r="A26" s="12"/>
     </row>
-    <row r="27" spans="1:14" ht="15.75" customHeight="1">
+    <row r="27" spans="1:14" ht="26.4">
       <c r="A27" s="20" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1">
@@ -2103,13 +2103,13 @@
         <v>16</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="5" t="s">
@@ -2131,15 +2131,15 @@
         <v>18</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s">
         <v>16</v>
@@ -2157,7 +2157,7 @@
         <v>18</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>18</v>
@@ -2175,12 +2175,12 @@
         <v>18</v>
       </c>
       <c r="N29" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B30" s="19" t="s">
         <v>42</v>
@@ -2201,7 +2201,7 @@
         <v>18</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I30" s="5" t="s">
         <v>18</v>
@@ -2219,15 +2219,15 @@
         <v>18</v>
       </c>
       <c r="N30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
         <v>16</v>
@@ -2245,7 +2245,7 @@
         <v>18</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>18</v>
@@ -2263,24 +2263,24 @@
         <v>18</v>
       </c>
       <c r="N31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F32" t="s">
         <v>18</v>
@@ -2289,7 +2289,7 @@
         <v>18</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>18</v>
@@ -2307,15 +2307,15 @@
         <v>18</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="13.2">
       <c r="A34" s="12"/>
     </row>
-    <row r="35" spans="1:14" ht="13.2">
+    <row r="35" spans="1:14" ht="26.4">
       <c r="A35" s="20" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.2">
@@ -2328,20 +2328,18 @@
       <c r="C36" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="G36" s="22"/>
+      <c r="H36" t="s">
         <v>129</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" t="s">
-        <v>132</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>18</v>
@@ -2359,33 +2357,33 @@
         <v>18</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.2">
       <c r="A37" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D37" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" t="s">
         <v>129</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="F37" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" t="s">
-        <v>132</v>
       </c>
       <c r="I37" s="5" t="s">
         <v>18</v>
@@ -2403,42 +2401,42 @@
         <v>18</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.2">
       <c r="A38" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G38" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H38" s="22" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>18</v>
@@ -2447,12 +2445,12 @@
         <v>18</v>
       </c>
       <c r="N38" s="22" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="13.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="26.4">
       <c r="A39" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B39" s="19" t="s">
         <v>42</v>
@@ -2460,46 +2458,46 @@
       <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F39" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" t="s">
-        <v>18</v>
+      <c r="D39" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>46</v>
       </c>
       <c r="H39" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M39" s="5" t="s">
-        <v>18</v>
+      <c r="J39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="M39" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="N39" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.2">
       <c r="A40" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>19</v>
@@ -2517,7 +2515,7 @@
         <v>18</v>
       </c>
       <c r="H40" s="22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>18</v>
@@ -2535,51 +2533,51 @@
         <v>18</v>
       </c>
       <c r="N40" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.2">
       <c r="A41" s="24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H41" s="22" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>18</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="K41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="N41" s="22" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.2">
@@ -5423,14 +5421,14 @@
     <hyperlink ref="B28" r:id="rId32" location="evt_system_boot" xr:uid="{66ACADCD-3286-477A-ABB6-57512EE79561}"/>
     <hyperlink ref="B32" r:id="rId33" location="evt_le_connection_closed" xr:uid="{FB973842-DC54-4C76-84D5-3409E68323AB}"/>
     <hyperlink ref="E32" r:id="rId34" location="cmd_sm_delete_bondings" xr:uid="{A96C6D10-B410-4765-A2A6-C6564A3DDCB3}"/>
-    <hyperlink ref="E36" r:id="rId35" location="cmd_sm_delete_bondings" xr:uid="{A01D8C18-6439-45BE-81B7-65158E72E312}"/>
-    <hyperlink ref="E37" r:id="rId36" location="cmd_sm_delete_bondings" xr:uid="{8B744716-267D-47D0-97D6-2EE5FCB08993}"/>
-    <hyperlink ref="B38" r:id="rId37" location="evt_sm_confirm_passkey" xr:uid="{5F8A14A8-0FD8-4BEC-AA20-0FB0AFE6E548}"/>
-    <hyperlink ref="B39" r:id="rId38" location="evt_sm_bonded" xr:uid="{A82A361A-E810-4617-A1A7-7114B1A0B58E}"/>
-    <hyperlink ref="B40" r:id="rId39" location="evt_sm_bonding_failed" xr:uid="{FD30E1A7-EF75-4420-ADE2-4EF277C9E698}"/>
-    <hyperlink ref="B37" r:id="rId40" location="evt_le_connection_closed" xr:uid="{04A92649-A104-4A56-B2F8-826286EE6A7A}"/>
-    <hyperlink ref="B36" r:id="rId41" location="evt_system_boot" xr:uid="{8312EAFF-6A90-4703-87FD-4A9FB12B4644}"/>
-    <hyperlink ref="B41" r:id="rId42" location="evt_gatt_characteristic_value" xr:uid="{A843C51F-02F1-40CB-ABA5-5B08C15B7C97}"/>
+    <hyperlink ref="E37" r:id="rId35" location="cmd_sm_delete_bondings" xr:uid="{8B744716-267D-47D0-97D6-2EE5FCB08993}"/>
+    <hyperlink ref="B38" r:id="rId36" location="evt_sm_confirm_passkey" xr:uid="{5F8A14A8-0FD8-4BEC-AA20-0FB0AFE6E548}"/>
+    <hyperlink ref="B39" r:id="rId37" location="evt_sm_bonded" xr:uid="{A82A361A-E810-4617-A1A7-7114B1A0B58E}"/>
+    <hyperlink ref="B40" r:id="rId38" location="evt_sm_bonding_failed" xr:uid="{FD30E1A7-EF75-4420-ADE2-4EF277C9E698}"/>
+    <hyperlink ref="B37" r:id="rId39" location="evt_le_connection_closed" xr:uid="{04A92649-A104-4A56-B2F8-826286EE6A7A}"/>
+    <hyperlink ref="B36" r:id="rId40" location="evt_system_boot" xr:uid="{8312EAFF-6A90-4703-87FD-4A9FB12B4644}"/>
+    <hyperlink ref="B41" r:id="rId41" location="evt_gatt_characteristic_value" xr:uid="{A843C51F-02F1-40CB-ABA5-5B08C15B7C97}"/>
+    <hyperlink ref="E39" r:id="rId42" location="cmd_gatt_discover_primary_services_by_uuid" xr:uid="{D340FE65-F867-4BA4-B9D2-F1765C4ED0BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId43"/>

</xml_diff>